<commit_message>
segregated the women all file and adding some rec of errors file from women
</commit_message>
<xml_diff>
--- a/Extraction/assets/real_real_urls/real_real_women_watches.xlsx
+++ b/Extraction/assets/real_real_urls/real_real_women_watches.xlsx
@@ -6008,7 +6008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1883"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>